<commit_message>
Downloaded latest bond data from Box
</commit_message>
<xml_diff>
--- a/DATA/RAW/bond_data/os_PA3540038_Schuylkill.xlsx
+++ b/DATA/RAW/bond_data/os_PA3540038_Schuylkill.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19524\Box\Shrinking Cities\data\bond_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19524\Box\Shrinking Cities MP\data\bond_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11E5947-0775-472C-9655-1E87CA0E8432}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC89B479-5D97-4774-A590-4D23BE3BA543}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="11" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="notes" sheetId="17" r:id="rId1"/>
@@ -33,6 +33,7 @@
     <sheet name="fiscal" sheetId="16" r:id="rId18"/>
     <sheet name="assets" sheetId="20" r:id="rId19"/>
     <sheet name="revCollect" sheetId="15" r:id="rId20"/>
+    <sheet name="financialIndicators" sheetId="21" r:id="rId21"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -50,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5997" uniqueCount="611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6070" uniqueCount="671">
   <si>
     <t>PWSID</t>
   </si>
@@ -1883,18 +1886,355 @@
   </si>
   <si>
     <t>Refunding Requirement - 2015 bonds (these bonds were acquired with the Butler Township Municipal Authority)</t>
+  </si>
+  <si>
+    <t>Line Item</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>[1]</t>
+  </si>
+  <si>
+    <t>Enter as shown in the Total Operating Revenues line</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>[2]</t>
+  </si>
+  <si>
+    <t>Enter as shown in the Total Operating Expenses line</t>
+  </si>
+  <si>
+    <t>[3]</t>
+  </si>
+  <si>
+    <t>Depreciation &amp; Amortization Expenses</t>
+  </si>
+  <si>
+    <t>Depreciation and amortization are listed as a line item within Operating Expenses</t>
+  </si>
+  <si>
+    <t>[4]</t>
+  </si>
+  <si>
+    <t>Debt Principal Payments</t>
+  </si>
+  <si>
+    <t>Enter $0 if there were no debt service payments</t>
+  </si>
+  <si>
+    <t>[4b]</t>
+  </si>
+  <si>
+    <t>Debt Interest Payments</t>
+  </si>
+  <si>
+    <t>[5]</t>
+  </si>
+  <si>
+    <t>Current Assets, excluding inventories, restricted cash, prepaids</t>
+  </si>
+  <si>
+    <t>Total Current Assets minus all inventories, prepaid items and any kind of restricted cash or restricted assets that cannot be used to pay for Current Liabilities</t>
+  </si>
+  <si>
+    <t>[6]</t>
+  </si>
+  <si>
+    <t>Current Liabilities, excluding deposits &amp; bond anticipation notes</t>
+  </si>
+  <si>
+    <t>Total Current Liabilities minus all refundable deposits and bond anticipation notes</t>
+  </si>
+  <si>
+    <t>[7]</t>
+  </si>
+  <si>
+    <t>Unrestricted Cash &amp; Investments</t>
+  </si>
+  <si>
+    <t>Unrestricted Cash &amp; Investments (and Cash Equivalents) is listed as a line item within Current Assets</t>
+  </si>
+  <si>
+    <t>[8]</t>
+  </si>
+  <si>
+    <t>Total Accumulated Depreciation</t>
+  </si>
+  <si>
+    <t>Total accumulated depreciation on capital assets being depreciated (buildings, equipment, other improvements) is usually shown in the Detail Notes on Capital Assets.</t>
+  </si>
+  <si>
+    <t>[9]</t>
+  </si>
+  <si>
+    <t>Total Depreciable Capital Assets</t>
+  </si>
+  <si>
+    <t>Enter the total value of capital assets being depreciated (buildings, equipment, othre improvements) only. Often listed in Detail Notes on Capital Assets.</t>
+  </si>
+  <si>
+    <t>[10]</t>
+  </si>
+  <si>
+    <t>[11]</t>
+  </si>
+  <si>
+    <t>[12]</t>
+  </si>
+  <si>
+    <t>Capital Spending</t>
+  </si>
+  <si>
+    <t>Enter Current PPE less Prior PPE + Depreciation</t>
+  </si>
+  <si>
+    <t>Indicators</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>Operating Ratio (including depreciation)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">_[1]_ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+[2]</t>
+    </r>
+  </si>
+  <si>
+    <t>Operating Ratio (not including depreciation)</t>
+  </si>
+  <si>
+    <r>
+      <t>___</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[1]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">___
+ [2] - [3] </t>
+    </r>
+  </si>
+  <si>
+    <t>Debt Service coverage ratio</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">_[1] -  [2] + [3] _
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[4] + [4b]</t>
+    </r>
+  </si>
+  <si>
+    <t>Quick Ratio</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">_[5]_
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[6]</t>
+    </r>
+  </si>
+  <si>
+    <t>Days cash on hand</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">____[7]____
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(([2] - [3])/365)</t>
+    </r>
+  </si>
+  <si>
+    <t>Percent of capital assets depreciated</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">_[8]_
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[9]</t>
+    </r>
+  </si>
+  <si>
+    <t>Debt to Equity Ratio</t>
+  </si>
+  <si>
+    <r>
+      <t>__</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[11]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>__
+( [10] - [11])</t>
+    </r>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>Average plant age</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">_[8]_
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[3]</t>
+    </r>
+  </si>
+  <si>
+    <t>**</t>
+  </si>
+  <si>
+    <t>CapEx</t>
+  </si>
+  <si>
+    <t>Replacement ratio</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">_CapEx_
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[3]</t>
+    </r>
+  </si>
+  <si>
+    <t>*in cases where accumulated depcreciation is not available, calculate as: 35 - (net PPE / annual depreciation expense)</t>
+  </si>
+  <si>
+    <t>**can also look in cash flow statement for capex value</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="5">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1940,6 +2280,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1" tint="0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1979,12 +2349,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2035,11 +2406,40 @@
     <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -20421,17 +20821,17 @@
   <dimension ref="A1:AI45"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="Z3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E14" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="E2" sqref="E2"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AI3" sqref="AI3"/>
+      <selection pane="bottomRight" activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="3" width="8.88671875" style="1"/>
-    <col min="4" max="4" width="11.77734375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.44140625" style="1" customWidth="1"/>
     <col min="5" max="6" width="8.88671875" style="1"/>
     <col min="7" max="17" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="30" width="8.88671875" style="1"/>
@@ -24051,18 +24451,18 @@
   <dimension ref="A1:AI49"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="X14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="U3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
-      <selection pane="bottomRight" activeCell="AI49" sqref="AI49"/>
+      <selection pane="bottomRight" activeCell="AI6" sqref="AI6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="8.88671875" style="1"/>
     <col min="3" max="3" width="19.21875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" style="1" customWidth="1"/>
     <col min="5" max="6" width="8.88671875" style="1"/>
     <col min="7" max="7" width="12.109375" style="1" customWidth="1"/>
     <col min="8" max="34" width="8.88671875" style="1"/>
@@ -24260,8 +24660,8 @@
       <c r="AF3" s="13"/>
       <c r="AG3" s="13"/>
       <c r="AH3" s="13"/>
-      <c r="AI3" s="10" t="s">
-        <v>182</v>
+      <c r="AI3" s="10">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.3">
@@ -24309,8 +24709,8 @@
       <c r="AF4" s="13"/>
       <c r="AG4" s="13"/>
       <c r="AH4" s="13"/>
-      <c r="AI4" s="10" t="s">
-        <v>182</v>
+      <c r="AI4" s="10">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.3">
@@ -24358,8 +24758,8 @@
       <c r="AF5" s="13"/>
       <c r="AG5" s="13"/>
       <c r="AH5" s="13"/>
-      <c r="AI5" s="10" t="s">
-        <v>182</v>
+      <c r="AI5" s="10">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.3">
@@ -26769,6 +27169,2839 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46CD5F15-0435-4694-A994-75AAA1CD402C}">
+  <dimension ref="A1:AL38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6.88671875" customWidth="1"/>
+    <col min="2" max="2" width="61.109375" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="4" max="4" width="2.5546875" customWidth="1"/>
+    <col min="5" max="9" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="21" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="27" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="31" width="10" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="B1" s="28" t="s">
+        <v>611</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>612</v>
+      </c>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28">
+        <v>1986</v>
+      </c>
+      <c r="F1" s="28">
+        <v>1987</v>
+      </c>
+      <c r="G1" s="28">
+        <v>1988</v>
+      </c>
+      <c r="H1" s="28">
+        <v>1989</v>
+      </c>
+      <c r="I1" s="28">
+        <v>1990</v>
+      </c>
+      <c r="J1" s="28">
+        <v>1991</v>
+      </c>
+      <c r="K1" s="28">
+        <v>1992</v>
+      </c>
+      <c r="L1" s="28">
+        <v>1993</v>
+      </c>
+      <c r="M1" s="28">
+        <v>1994</v>
+      </c>
+      <c r="N1" s="28">
+        <v>1995</v>
+      </c>
+      <c r="O1" s="28">
+        <v>1996</v>
+      </c>
+      <c r="P1" s="28">
+        <v>1997</v>
+      </c>
+      <c r="Q1" s="28">
+        <v>1998</v>
+      </c>
+      <c r="R1" s="28">
+        <v>1999</v>
+      </c>
+      <c r="S1" s="28">
+        <v>2000</v>
+      </c>
+      <c r="T1" s="28">
+        <v>2001</v>
+      </c>
+      <c r="U1" s="28">
+        <v>2002</v>
+      </c>
+      <c r="V1" s="28">
+        <v>2003</v>
+      </c>
+      <c r="W1" s="28">
+        <v>2004</v>
+      </c>
+      <c r="X1" s="28">
+        <v>2005</v>
+      </c>
+      <c r="Y1" s="28">
+        <v>2006</v>
+      </c>
+      <c r="Z1" s="28">
+        <v>2007</v>
+      </c>
+      <c r="AA1" s="28">
+        <v>2008</v>
+      </c>
+      <c r="AB1" s="28">
+        <v>2009</v>
+      </c>
+      <c r="AC1" s="28">
+        <v>2010</v>
+      </c>
+      <c r="AD1" s="28">
+        <v>2011</v>
+      </c>
+      <c r="AE1" s="28">
+        <v>2012</v>
+      </c>
+      <c r="AF1" s="28">
+        <v>2013</v>
+      </c>
+      <c r="AG1" s="28">
+        <v>2014</v>
+      </c>
+      <c r="AH1" s="28">
+        <v>2015</v>
+      </c>
+      <c r="AI1" s="28">
+        <v>2016</v>
+      </c>
+      <c r="AJ1" s="28">
+        <v>2017</v>
+      </c>
+      <c r="AK1" s="28">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>613</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>614</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>615</v>
+      </c>
+      <c r="I2">
+        <f>fiscal!G14</f>
+        <v>2046181</v>
+      </c>
+      <c r="J2">
+        <f>fiscal!H14</f>
+        <v>2854984</v>
+      </c>
+      <c r="K2">
+        <f>fiscal!I14</f>
+        <v>3359292</v>
+      </c>
+      <c r="L2">
+        <f>fiscal!J14</f>
+        <v>3352876</v>
+      </c>
+      <c r="M2">
+        <f>fiscal!K14</f>
+        <v>4300682</v>
+      </c>
+      <c r="N2">
+        <f>fiscal!L14</f>
+        <v>4567193</v>
+      </c>
+      <c r="O2">
+        <f>fiscal!M14</f>
+        <v>4518027</v>
+      </c>
+      <c r="P2">
+        <f>fiscal!N14</f>
+        <v>4570539</v>
+      </c>
+      <c r="Q2">
+        <f>fiscal!O14</f>
+        <v>4566690</v>
+      </c>
+      <c r="R2">
+        <f>fiscal!P14</f>
+        <v>4727184</v>
+      </c>
+      <c r="S2">
+        <f>fiscal!Q14</f>
+        <v>4544985</v>
+      </c>
+      <c r="T2">
+        <f>fiscal!R14</f>
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <f>fiscal!S14</f>
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <f>fiscal!T14</f>
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <f>fiscal!U14</f>
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <f>fiscal!V14</f>
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <f>fiscal!W14</f>
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <f>fiscal!X14</f>
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <f>fiscal!Y14</f>
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <f>fiscal!Z14</f>
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <f>fiscal!AA14</f>
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <f>fiscal!AB14</f>
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <f>fiscal!AC14</f>
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <f>fiscal!AD14</f>
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <f>fiscal!AE14</f>
+        <v>8224271</v>
+      </c>
+      <c r="AH2">
+        <f>fiscal!AF14</f>
+        <v>8326929</v>
+      </c>
+      <c r="AI2">
+        <f>fiscal!AG14</f>
+        <v>10159109</v>
+      </c>
+      <c r="AJ2">
+        <f>fiscal!AH14</f>
+        <v>10276811</v>
+      </c>
+      <c r="AK2">
+        <f>fiscal!AI14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>616</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>617</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>615</v>
+      </c>
+      <c r="I3">
+        <f>fiscal!G25</f>
+        <v>854798</v>
+      </c>
+      <c r="J3">
+        <f>fiscal!H25</f>
+        <v>958056</v>
+      </c>
+      <c r="K3">
+        <f>fiscal!I25</f>
+        <v>1246817</v>
+      </c>
+      <c r="L3">
+        <f>fiscal!J25</f>
+        <v>1312350</v>
+      </c>
+      <c r="M3">
+        <f>fiscal!K25</f>
+        <v>1506010</v>
+      </c>
+      <c r="N3">
+        <f>fiscal!L25</f>
+        <v>1527158</v>
+      </c>
+      <c r="O3">
+        <f>fiscal!M25</f>
+        <v>1681544</v>
+      </c>
+      <c r="P3">
+        <f>fiscal!N25</f>
+        <v>1645673</v>
+      </c>
+      <c r="Q3">
+        <f>fiscal!O25</f>
+        <v>1805262</v>
+      </c>
+      <c r="R3">
+        <f>fiscal!P25</f>
+        <v>1993775</v>
+      </c>
+      <c r="S3">
+        <f>fiscal!Q25</f>
+        <v>1967847</v>
+      </c>
+      <c r="T3">
+        <f>fiscal!R25</f>
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <f>fiscal!S25</f>
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <f>fiscal!T25</f>
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <f>fiscal!U25</f>
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <f>fiscal!V25</f>
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <f>fiscal!W25</f>
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <f>fiscal!X25</f>
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <f>fiscal!Y25</f>
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <f>fiscal!Z25</f>
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <f>fiscal!AA25</f>
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <f>fiscal!AB25</f>
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <f>fiscal!AC25</f>
+        <v>0</v>
+      </c>
+      <c r="AF3">
+        <f>fiscal!AD25</f>
+        <v>0</v>
+      </c>
+      <c r="AG3">
+        <f>fiscal!AE25</f>
+        <v>5636933</v>
+      </c>
+      <c r="AH3">
+        <f>fiscal!AF25</f>
+        <v>5780142</v>
+      </c>
+      <c r="AI3">
+        <f>fiscal!AG25</f>
+        <v>6116965</v>
+      </c>
+      <c r="AJ3">
+        <f>fiscal!AH25</f>
+        <v>7704290</v>
+      </c>
+      <c r="AK3">
+        <f>fiscal!AI25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>618</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>619</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>620</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>615</v>
+      </c>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="31"/>
+      <c r="P4" s="31"/>
+      <c r="Q4" s="31"/>
+      <c r="R4" s="31"/>
+      <c r="S4" s="31"/>
+      <c r="T4" s="31"/>
+      <c r="U4" s="31"/>
+      <c r="V4" s="31"/>
+      <c r="W4" s="31"/>
+      <c r="X4" s="31"/>
+      <c r="Y4" s="31"/>
+      <c r="Z4" s="31"/>
+      <c r="AA4" s="31"/>
+      <c r="AB4" s="31"/>
+      <c r="AC4" s="31"/>
+      <c r="AD4" s="31"/>
+      <c r="AE4" s="31"/>
+      <c r="AF4" s="31"/>
+      <c r="AG4" s="31"/>
+      <c r="AH4" s="31"/>
+      <c r="AI4" s="31"/>
+      <c r="AJ4" s="31"/>
+      <c r="AK4" s="31"/>
+    </row>
+    <row r="5" spans="1:37" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>621</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>622</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>623</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>624</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>625</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>623</v>
+      </c>
+      <c r="D6" s="30" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>626</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>627</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>628</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>615</v>
+      </c>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31">
+        <f>assets!G12-assets!G6-assets!G5</f>
+        <v>1109311</v>
+      </c>
+      <c r="J7" s="31">
+        <f>assets!H12-assets!H6-assets!H5</f>
+        <v>0</v>
+      </c>
+      <c r="K7" s="31">
+        <f>assets!I12-assets!I6-assets!I5</f>
+        <v>0</v>
+      </c>
+      <c r="L7" s="31">
+        <f>assets!J12-assets!J6-assets!J5</f>
+        <v>0</v>
+      </c>
+      <c r="M7" s="31">
+        <f>assets!K12-assets!K6-assets!K5</f>
+        <v>0</v>
+      </c>
+      <c r="N7" s="31">
+        <f>assets!L12-assets!L6-assets!L5</f>
+        <v>0</v>
+      </c>
+      <c r="O7" s="31">
+        <f>assets!M12-assets!M6-assets!M5</f>
+        <v>0</v>
+      </c>
+      <c r="P7" s="31">
+        <f>assets!N12-assets!N6-assets!N5</f>
+        <v>0</v>
+      </c>
+      <c r="Q7" s="31">
+        <f>assets!O12-assets!O6-assets!O5</f>
+        <v>0</v>
+      </c>
+      <c r="R7" s="31">
+        <f>assets!P12-assets!P6-assets!P5</f>
+        <v>0</v>
+      </c>
+      <c r="S7" s="31">
+        <f>assets!Q12-assets!Q6-assets!Q5</f>
+        <v>0</v>
+      </c>
+      <c r="T7" s="31">
+        <f>assets!R12-assets!R6-assets!R5</f>
+        <v>0</v>
+      </c>
+      <c r="U7" s="31">
+        <f>assets!S12-assets!S6-assets!S5</f>
+        <v>0</v>
+      </c>
+      <c r="V7" s="31">
+        <f>assets!T12-assets!T6-assets!T5</f>
+        <v>0</v>
+      </c>
+      <c r="W7" s="31">
+        <f>assets!U12-assets!U6-assets!U5</f>
+        <v>0</v>
+      </c>
+      <c r="X7" s="31">
+        <f>assets!V12-assets!V6-assets!V5</f>
+        <v>0</v>
+      </c>
+      <c r="Y7" s="31">
+        <f>assets!W12-assets!W6-assets!W5</f>
+        <v>0</v>
+      </c>
+      <c r="Z7" s="31">
+        <f>assets!X12-assets!X6-assets!X5</f>
+        <v>0</v>
+      </c>
+      <c r="AA7" s="31">
+        <f>assets!Y12-assets!Y6-assets!Y5</f>
+        <v>0</v>
+      </c>
+      <c r="AB7" s="31">
+        <f>assets!Z12-assets!Z6-assets!Z5</f>
+        <v>0</v>
+      </c>
+      <c r="AC7" s="31">
+        <f>assets!AA12-assets!AA6-assets!AA5</f>
+        <v>0</v>
+      </c>
+      <c r="AD7" s="31">
+        <f>assets!AB12-assets!AB6-assets!AB5</f>
+        <v>0</v>
+      </c>
+      <c r="AE7" s="31">
+        <f>assets!AC12-assets!AC6-assets!AC5</f>
+        <v>0</v>
+      </c>
+      <c r="AF7" s="31">
+        <f>assets!AD12-assets!AD6-assets!AD5</f>
+        <v>0</v>
+      </c>
+      <c r="AG7" s="31">
+        <f>assets!AE12-assets!AE6-assets!AE5</f>
+        <v>0</v>
+      </c>
+      <c r="AH7" s="31">
+        <f>assets!AF12-assets!AF6-assets!AF5</f>
+        <v>0</v>
+      </c>
+      <c r="AI7" s="31">
+        <f>assets!AG12-assets!AG6-assets!AG5</f>
+        <v>0</v>
+      </c>
+      <c r="AJ7" s="31">
+        <f>assets!AH12-assets!AH6-assets!AH5</f>
+        <v>0</v>
+      </c>
+      <c r="AK7" s="31">
+        <f>assets!AI12-assets!AI6-assets!AI5</f>
+        <v>11474657</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>629</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>630</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>631</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>615</v>
+      </c>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31">
+        <f>assets!G36-assets!G30</f>
+        <v>975</v>
+      </c>
+      <c r="J8" s="31">
+        <f>assets!H36-assets!H30</f>
+        <v>0</v>
+      </c>
+      <c r="K8" s="31">
+        <f>assets!I36-assets!I30</f>
+        <v>0</v>
+      </c>
+      <c r="L8" s="31">
+        <f>assets!J36-assets!J30</f>
+        <v>0</v>
+      </c>
+      <c r="M8" s="31">
+        <f>assets!K36-assets!K30</f>
+        <v>0</v>
+      </c>
+      <c r="N8" s="31">
+        <f>assets!L36-assets!L30</f>
+        <v>0</v>
+      </c>
+      <c r="O8" s="31">
+        <f>assets!M36-assets!M30</f>
+        <v>0</v>
+      </c>
+      <c r="P8" s="31">
+        <f>assets!N36-assets!N30</f>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="31">
+        <f>assets!O36-assets!O30</f>
+        <v>0</v>
+      </c>
+      <c r="R8" s="31">
+        <f>assets!P36-assets!P30</f>
+        <v>0</v>
+      </c>
+      <c r="S8" s="31">
+        <f>assets!Q36-assets!Q30</f>
+        <v>0</v>
+      </c>
+      <c r="T8" s="31">
+        <f>assets!R36-assets!R30</f>
+        <v>0</v>
+      </c>
+      <c r="U8" s="31">
+        <f>assets!S36-assets!S30</f>
+        <v>0</v>
+      </c>
+      <c r="V8" s="31">
+        <f>assets!T36-assets!T30</f>
+        <v>0</v>
+      </c>
+      <c r="W8" s="31">
+        <f>assets!U36-assets!U30</f>
+        <v>0</v>
+      </c>
+      <c r="X8" s="31">
+        <f>assets!V36-assets!V30</f>
+        <v>0</v>
+      </c>
+      <c r="Y8" s="31">
+        <f>assets!W36-assets!W30</f>
+        <v>0</v>
+      </c>
+      <c r="Z8" s="31">
+        <f>assets!X36-assets!X30</f>
+        <v>0</v>
+      </c>
+      <c r="AA8" s="31">
+        <f>assets!Y36-assets!Y30</f>
+        <v>0</v>
+      </c>
+      <c r="AB8" s="31">
+        <f>assets!Z36-assets!Z30</f>
+        <v>0</v>
+      </c>
+      <c r="AC8" s="31">
+        <f>assets!AA36-assets!AA30</f>
+        <v>0</v>
+      </c>
+      <c r="AD8" s="31">
+        <f>assets!AB36-assets!AB30</f>
+        <v>0</v>
+      </c>
+      <c r="AE8" s="31">
+        <f>assets!AC36-assets!AC30</f>
+        <v>0</v>
+      </c>
+      <c r="AF8" s="31">
+        <f>assets!AD36-assets!AD30</f>
+        <v>0</v>
+      </c>
+      <c r="AG8" s="31">
+        <f>assets!AE36-assets!AE30</f>
+        <v>0</v>
+      </c>
+      <c r="AH8" s="31">
+        <f>assets!AF36-assets!AF30</f>
+        <v>0</v>
+      </c>
+      <c r="AI8" s="31">
+        <f>assets!AG36-assets!AG30</f>
+        <v>0</v>
+      </c>
+      <c r="AJ8" s="31">
+        <f>assets!AH36-assets!AH30</f>
+        <v>0</v>
+      </c>
+      <c r="AK8" s="31">
+        <f>assets!AI36-assets!AI30</f>
+        <v>2803536</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>632</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>633</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>634</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>615</v>
+      </c>
+      <c r="I9">
+        <f>assets!G3+assets!G4</f>
+        <v>1099311</v>
+      </c>
+      <c r="J9">
+        <f>assets!H3+assets!H4</f>
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <f>assets!I3+assets!I4</f>
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <f>assets!J3+assets!J4</f>
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <f>assets!K3+assets!K4</f>
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <f>assets!L3+assets!L4</f>
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <f>assets!M3+assets!M4</f>
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <f>assets!N3+assets!N4</f>
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <f>assets!O3+assets!O4</f>
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <f>assets!P3+assets!P4</f>
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <f>assets!Q3+assets!Q4</f>
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <f>assets!R3+assets!R4</f>
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <f>assets!S3+assets!S4</f>
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <f>assets!T3+assets!T4</f>
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <f>assets!U3+assets!U4</f>
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <f>assets!V3+assets!V4</f>
+        <v>0</v>
+      </c>
+      <c r="Y9">
+        <f>assets!W3+assets!W4</f>
+        <v>0</v>
+      </c>
+      <c r="Z9">
+        <f>assets!X3+assets!X4</f>
+        <v>0</v>
+      </c>
+      <c r="AA9">
+        <f>assets!Y3+assets!Y4</f>
+        <v>0</v>
+      </c>
+      <c r="AB9">
+        <f>assets!Z3+assets!Z4</f>
+        <v>0</v>
+      </c>
+      <c r="AC9">
+        <f>assets!AA3+assets!AA4</f>
+        <v>0</v>
+      </c>
+      <c r="AD9">
+        <f>assets!AB3+assets!AB4</f>
+        <v>0</v>
+      </c>
+      <c r="AE9">
+        <f>assets!AC3+assets!AC4</f>
+        <v>0</v>
+      </c>
+      <c r="AF9">
+        <f>assets!AD3+assets!AD4</f>
+        <v>0</v>
+      </c>
+      <c r="AG9">
+        <f>assets!AE3+assets!AE4</f>
+        <v>0</v>
+      </c>
+      <c r="AH9">
+        <f>assets!AF3+assets!AF4</f>
+        <v>0</v>
+      </c>
+      <c r="AI9">
+        <f>assets!AG3+assets!AG4</f>
+        <v>0</v>
+      </c>
+      <c r="AJ9">
+        <f>assets!AH3+assets!AH4</f>
+        <v>0</v>
+      </c>
+      <c r="AK9">
+        <f>assets!AI3+assets!AI4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>635</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>636</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>637</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>615</v>
+      </c>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="31"/>
+      <c r="O10" s="31"/>
+      <c r="P10" s="31"/>
+      <c r="Q10" s="31"/>
+      <c r="R10" s="31"/>
+      <c r="S10" s="31"/>
+      <c r="T10" s="31"/>
+      <c r="U10" s="31"/>
+      <c r="V10" s="31"/>
+      <c r="W10" s="31"/>
+      <c r="X10" s="31"/>
+      <c r="Y10" s="31"/>
+      <c r="Z10" s="31"/>
+      <c r="AA10" s="31"/>
+      <c r="AB10" s="31"/>
+      <c r="AC10" s="31"/>
+      <c r="AD10" s="31"/>
+      <c r="AE10" s="31"/>
+      <c r="AF10" s="31"/>
+      <c r="AG10" s="31"/>
+      <c r="AH10" s="31"/>
+      <c r="AI10" s="31"/>
+      <c r="AJ10" s="31"/>
+      <c r="AK10" s="31"/>
+    </row>
+    <row r="11" spans="1:37" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>638</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>639</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>640</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>615</v>
+      </c>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32">
+        <f>assets!G19</f>
+        <v>17405222</v>
+      </c>
+      <c r="J11" s="32">
+        <f>assets!H19</f>
+        <v>0</v>
+      </c>
+      <c r="K11" s="32">
+        <f>assets!I19</f>
+        <v>0</v>
+      </c>
+      <c r="L11" s="32">
+        <f>assets!J19</f>
+        <v>0</v>
+      </c>
+      <c r="M11" s="32">
+        <f>assets!K19</f>
+        <v>0</v>
+      </c>
+      <c r="N11" s="32">
+        <f>assets!L19</f>
+        <v>0</v>
+      </c>
+      <c r="O11" s="32">
+        <f>assets!M19</f>
+        <v>0</v>
+      </c>
+      <c r="P11" s="32">
+        <f>assets!N19</f>
+        <v>0</v>
+      </c>
+      <c r="Q11" s="32">
+        <f>assets!O19</f>
+        <v>0</v>
+      </c>
+      <c r="R11" s="32">
+        <f>assets!P19</f>
+        <v>0</v>
+      </c>
+      <c r="S11" s="32">
+        <f>assets!Q19</f>
+        <v>0</v>
+      </c>
+      <c r="T11" s="32">
+        <f>assets!R19</f>
+        <v>0</v>
+      </c>
+      <c r="U11" s="32">
+        <f>assets!S19</f>
+        <v>0</v>
+      </c>
+      <c r="V11" s="32">
+        <f>assets!T19</f>
+        <v>0</v>
+      </c>
+      <c r="W11" s="32">
+        <f>assets!U19</f>
+        <v>0</v>
+      </c>
+      <c r="X11" s="32">
+        <f>assets!V19</f>
+        <v>0</v>
+      </c>
+      <c r="Y11" s="32">
+        <f>assets!W19</f>
+        <v>0</v>
+      </c>
+      <c r="Z11" s="32">
+        <f>assets!X19</f>
+        <v>0</v>
+      </c>
+      <c r="AA11" s="32">
+        <f>assets!Y19</f>
+        <v>0</v>
+      </c>
+      <c r="AB11" s="32">
+        <f>assets!Z19</f>
+        <v>0</v>
+      </c>
+      <c r="AC11" s="32">
+        <f>assets!AA19</f>
+        <v>0</v>
+      </c>
+      <c r="AD11" s="32">
+        <f>assets!AB19</f>
+        <v>0</v>
+      </c>
+      <c r="AE11" s="32">
+        <f>assets!AC19</f>
+        <v>0</v>
+      </c>
+      <c r="AF11" s="32">
+        <f>assets!AD19</f>
+        <v>0</v>
+      </c>
+      <c r="AG11" s="32">
+        <f>assets!AE19</f>
+        <v>0</v>
+      </c>
+      <c r="AH11" s="32">
+        <f>assets!AF19</f>
+        <v>0</v>
+      </c>
+      <c r="AI11" s="32">
+        <f>assets!AG19</f>
+        <v>0</v>
+      </c>
+      <c r="AJ11" s="32">
+        <f>assets!AH19</f>
+        <v>0</v>
+      </c>
+      <c r="AK11" s="32">
+        <f>assets!AI19</f>
+        <v>91821360</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>641</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>163</v>
+      </c>
+      <c r="I12">
+        <f>assets!G29</f>
+        <v>19628535</v>
+      </c>
+      <c r="J12">
+        <f>assets!H29</f>
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <f>assets!I29</f>
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <f>assets!J29</f>
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <f>assets!K29</f>
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <f>assets!L29</f>
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <f>assets!M29</f>
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <f>assets!N29</f>
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <f>assets!O29</f>
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <f>assets!P29</f>
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <f>assets!Q29</f>
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <f>assets!R29</f>
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <f>assets!S29</f>
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <f>assets!T29</f>
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <f>assets!U29</f>
+        <v>0</v>
+      </c>
+      <c r="X12">
+        <f>assets!V29</f>
+        <v>0</v>
+      </c>
+      <c r="Y12">
+        <f>assets!W29</f>
+        <v>0</v>
+      </c>
+      <c r="Z12">
+        <f>assets!X29</f>
+        <v>0</v>
+      </c>
+      <c r="AA12">
+        <f>assets!Y29</f>
+        <v>0</v>
+      </c>
+      <c r="AB12">
+        <f>assets!Z29</f>
+        <v>0</v>
+      </c>
+      <c r="AC12">
+        <f>assets!AA29</f>
+        <v>0</v>
+      </c>
+      <c r="AD12">
+        <f>assets!AB29</f>
+        <v>0</v>
+      </c>
+      <c r="AE12">
+        <f>assets!AC29</f>
+        <v>0</v>
+      </c>
+      <c r="AF12">
+        <f>assets!AD29</f>
+        <v>0</v>
+      </c>
+      <c r="AG12">
+        <f>assets!AE29</f>
+        <v>0</v>
+      </c>
+      <c r="AH12">
+        <f>assets!AF29</f>
+        <v>0</v>
+      </c>
+      <c r="AI12">
+        <f>assets!AG29</f>
+        <v>0</v>
+      </c>
+      <c r="AJ12">
+        <f>assets!AH29</f>
+        <v>0</v>
+      </c>
+      <c r="AK12">
+        <f>assets!AI29</f>
+        <v>103514752</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>642</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>166</v>
+      </c>
+      <c r="I13">
+        <f>assets!G43</f>
+        <v>4968366</v>
+      </c>
+      <c r="J13">
+        <f>assets!H43</f>
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <f>assets!I43</f>
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <f>assets!J43</f>
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <f>assets!K43</f>
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <f>assets!L43</f>
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <f>assets!M43</f>
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <f>assets!N43</f>
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <f>assets!O43</f>
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <f>assets!P43</f>
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <f>assets!Q43</f>
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <f>assets!R43</f>
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <f>assets!S43</f>
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <f>assets!T43</f>
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <f>assets!U43</f>
+        <v>0</v>
+      </c>
+      <c r="X13">
+        <f>assets!V43</f>
+        <v>0</v>
+      </c>
+      <c r="Y13">
+        <f>assets!W43</f>
+        <v>0</v>
+      </c>
+      <c r="Z13">
+        <f>assets!X43</f>
+        <v>0</v>
+      </c>
+      <c r="AA13">
+        <f>assets!Y43</f>
+        <v>0</v>
+      </c>
+      <c r="AB13">
+        <f>assets!Z43</f>
+        <v>0</v>
+      </c>
+      <c r="AC13">
+        <f>assets!AA43</f>
+        <v>0</v>
+      </c>
+      <c r="AD13">
+        <f>assets!AB43</f>
+        <v>0</v>
+      </c>
+      <c r="AE13">
+        <f>assets!AC43</f>
+        <v>0</v>
+      </c>
+      <c r="AF13">
+        <f>assets!AD43</f>
+        <v>0</v>
+      </c>
+      <c r="AG13">
+        <f>assets!AE43</f>
+        <v>0</v>
+      </c>
+      <c r="AH13">
+        <f>assets!AF43</f>
+        <v>0</v>
+      </c>
+      <c r="AI13">
+        <f>assets!AG43</f>
+        <v>0</v>
+      </c>
+      <c r="AJ13">
+        <f>assets!AH43</f>
+        <v>0</v>
+      </c>
+      <c r="AK13">
+        <f>assets!AI43</f>
+        <v>40562365</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>643</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>644</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>645</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>615</v>
+      </c>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="32"/>
+      <c r="L14" s="32"/>
+      <c r="M14" s="32"/>
+      <c r="N14" s="32"/>
+      <c r="O14" s="32"/>
+      <c r="P14" s="32"/>
+      <c r="Q14" s="32"/>
+      <c r="R14" s="32"/>
+      <c r="S14" s="32"/>
+      <c r="T14" s="32"/>
+      <c r="U14" s="32"/>
+      <c r="V14" s="32"/>
+      <c r="W14" s="32"/>
+      <c r="X14" s="32"/>
+      <c r="Y14" s="32"/>
+      <c r="Z14" s="32"/>
+      <c r="AA14" s="32"/>
+      <c r="AB14" s="32"/>
+      <c r="AC14" s="32"/>
+      <c r="AD14" s="32"/>
+      <c r="AE14" s="32"/>
+      <c r="AF14" s="32"/>
+      <c r="AG14" s="32"/>
+      <c r="AH14" s="32"/>
+      <c r="AI14" s="32"/>
+      <c r="AJ14" s="32"/>
+      <c r="AK14" s="32"/>
+    </row>
+    <row r="16" spans="1:37" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B16" s="33" t="s">
+        <v>646</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>647</v>
+      </c>
+      <c r="D16" s="34"/>
+    </row>
+    <row r="17" spans="1:38" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>648</v>
+      </c>
+      <c r="C17" s="35" t="s">
+        <v>649</v>
+      </c>
+      <c r="D17" s="35"/>
+      <c r="E17" s="36" t="str">
+        <f>IFERROR(E2/E3, "")</f>
+        <v/>
+      </c>
+      <c r="F17" s="36" t="str">
+        <f t="shared" ref="F17:AK17" si="0">IFERROR(F2/F3, "")</f>
+        <v/>
+      </c>
+      <c r="G17" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H17" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I17" s="36">
+        <f t="shared" si="0"/>
+        <v>2.3937596952730353</v>
+      </c>
+      <c r="J17" s="36">
+        <f t="shared" si="0"/>
+        <v>2.979976118306237</v>
+      </c>
+      <c r="K17" s="36">
+        <f t="shared" si="0"/>
+        <v>2.6942943511357322</v>
+      </c>
+      <c r="L17" s="36">
+        <f t="shared" si="0"/>
+        <v>2.5548641749533281</v>
+      </c>
+      <c r="M17" s="36">
+        <f t="shared" si="0"/>
+        <v>2.8556795771608421</v>
+      </c>
+      <c r="N17" s="36">
+        <f t="shared" si="0"/>
+        <v>2.9906486427730465</v>
+      </c>
+      <c r="O17" s="36">
+        <f t="shared" si="0"/>
+        <v>2.6868324587403007</v>
+      </c>
+      <c r="P17" s="36">
+        <f t="shared" si="0"/>
+        <v>2.7773069133418367</v>
+      </c>
+      <c r="Q17" s="36">
+        <f t="shared" si="0"/>
+        <v>2.5296549752889055</v>
+      </c>
+      <c r="R17" s="36">
+        <f t="shared" si="0"/>
+        <v>2.3709716492583164</v>
+      </c>
+      <c r="S17" s="36">
+        <f t="shared" si="0"/>
+        <v>2.3096231566783394</v>
+      </c>
+      <c r="T17" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="U17" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="V17" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="W17" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="X17" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Y17" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Z17" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AA17" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AB17" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AC17" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AD17" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AE17" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AF17" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AG17" s="36">
+        <f t="shared" si="0"/>
+        <v>1.4589974725617636</v>
+      </c>
+      <c r="AH17" s="36">
+        <f t="shared" si="0"/>
+        <v>1.4406097635663622</v>
+      </c>
+      <c r="AI17" s="36">
+        <f t="shared" si="0"/>
+        <v>1.6608087507448548</v>
+      </c>
+      <c r="AJ17" s="36">
+        <f t="shared" si="0"/>
+        <v>1.3339076021281651</v>
+      </c>
+      <c r="AK17" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:38" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>650</v>
+      </c>
+      <c r="C18" s="35" t="s">
+        <v>651</v>
+      </c>
+      <c r="D18" s="35"/>
+      <c r="E18" s="36" t="str">
+        <f>IFERROR(IF(E4="","",E2/(E3-E4)), "")</f>
+        <v/>
+      </c>
+      <c r="F18" s="36" t="str">
+        <f t="shared" ref="F18:AK18" si="1">IFERROR(IF(F4="","",F2/(F3-F4)), "")</f>
+        <v/>
+      </c>
+      <c r="G18" s="36" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H18" s="36" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I18" s="36" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J18" s="36" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K18" s="36" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="L18" s="36" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="M18" s="36" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="N18" s="36" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="O18" s="36" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P18" s="36" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="Q18" s="36" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="R18" s="36" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="S18" s="36" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="T18" s="36" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="U18" s="36" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="V18" s="36" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="W18" s="36" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="X18" s="36" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="Y18" s="36" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="Z18" s="36" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="AA18" s="36" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="AB18" s="36" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="AC18" s="36" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="AD18" s="36" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="AE18" s="36" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="AF18" s="36" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="AG18" s="36" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="AH18" s="36" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="AI18" s="36" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="AJ18" s="36" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="AK18" s="36" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:38" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>652</v>
+      </c>
+      <c r="C19" s="37" t="s">
+        <v>653</v>
+      </c>
+      <c r="D19" s="37"/>
+      <c r="E19" s="36" t="str">
+        <f>IF(E4="","",IF(E5="","",IF(E6="","",(E2-E3+E4)/(E5+E6))))</f>
+        <v/>
+      </c>
+      <c r="F19" s="36" t="str">
+        <f t="shared" ref="F19:AK19" si="2">IF(F4="","",IF(F5="","",IF(F6="","",(F2-F3+F4)/(F5+F6))))</f>
+        <v/>
+      </c>
+      <c r="G19" s="36" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="H19" s="36" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I19" s="36" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J19" s="36" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K19" s="36" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L19" s="36" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="M19" s="36" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="N19" s="36" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="O19" s="36" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="P19" s="36" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="Q19" s="36" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="R19" s="36" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="S19" s="36" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="T19" s="36" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="U19" s="36" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="V19" s="36" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="W19" s="36" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="X19" s="36" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="Y19" s="36" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="Z19" s="36" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AA19" s="36" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AB19" s="36" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AC19" s="36" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AD19" s="36" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AE19" s="36" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AF19" s="36" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AG19" s="36" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AH19" s="36" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AI19" s="36" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AJ19" s="36" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AK19" s="36" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:38" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>654</v>
+      </c>
+      <c r="C20" s="37" t="s">
+        <v>655</v>
+      </c>
+      <c r="D20" s="37"/>
+      <c r="E20" s="36" t="str">
+        <f>IFERROR(E7/E8, "")</f>
+        <v/>
+      </c>
+      <c r="F20" s="36" t="str">
+        <f t="shared" ref="F20:AK20" si="3">IFERROR(F7/F8, "")</f>
+        <v/>
+      </c>
+      <c r="G20" s="36" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H20" s="36" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I20" s="36">
+        <f t="shared" si="3"/>
+        <v>1137.7548717948719</v>
+      </c>
+      <c r="J20" s="36" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="K20" s="36" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="L20" s="36" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M20" s="36" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="N20" s="36" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="O20" s="36" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="P20" s="36" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="Q20" s="36" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="R20" s="36" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="S20" s="36" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="T20" s="36" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="U20" s="36" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="V20" s="36" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="W20" s="36" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="X20" s="36" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="Y20" s="36" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="Z20" s="36" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="AA20" s="36" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="AB20" s="36" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="AC20" s="36" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="AD20" s="36" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="AE20" s="36" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="AF20" s="36" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="AG20" s="36" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="AH20" s="36" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="AI20" s="36" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="AJ20" s="36" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="AK20" s="36">
+        <f t="shared" si="3"/>
+        <v>4.092923008657638</v>
+      </c>
+    </row>
+    <row r="21" spans="1:38" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>656</v>
+      </c>
+      <c r="C21" s="37" t="s">
+        <v>657</v>
+      </c>
+      <c r="D21" s="37"/>
+      <c r="E21" s="38" t="str">
+        <f>IFERROR(IF(E9=0,"",IF(E4="","",IF(E9="","",E9/((E3-E4)/365)))),"")</f>
+        <v/>
+      </c>
+      <c r="F21" s="38" t="str">
+        <f t="shared" ref="F21:AK21" si="4">IFERROR(IF(F9=0,"",IF(F4="","",IF(F9="","",F9/((F3-F4)/365)))),"")</f>
+        <v/>
+      </c>
+      <c r="G21" s="38" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="H21" s="38" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="I21" s="38" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="J21" s="38" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K21" s="38" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L21" s="38" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="M21" s="38" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="N21" s="38" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="O21" s="38" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="P21" s="38" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Q21" s="38" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="R21" s="38" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="S21" s="38" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="T21" s="38" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="U21" s="38" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="V21" s="38" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="W21" s="38" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="X21" s="38" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Y21" s="38" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Z21" s="38" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AA21" s="38" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AB21" s="38" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AC21" s="38" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AD21" s="38" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AE21" s="38" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AF21" s="38" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AG21" s="38" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AH21" s="38" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AI21" s="38" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AJ21" s="38" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AK21" s="38" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:38" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>658</v>
+      </c>
+      <c r="C22" s="37" t="s">
+        <v>659</v>
+      </c>
+      <c r="D22" s="37"/>
+      <c r="E22" s="39" t="str">
+        <f>IFERROR(IF(E10="","",E10/E11), "")</f>
+        <v/>
+      </c>
+      <c r="F22" s="39" t="str">
+        <f t="shared" ref="F22:AL22" si="5">IFERROR(IF(F10="","",F10/F11), "")</f>
+        <v/>
+      </c>
+      <c r="G22" s="39" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="H22" s="39" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="I22" s="39" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="J22" s="39" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="K22" s="39" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="L22" s="39" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M22" s="39" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N22" s="39" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="O22" s="39" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="P22" s="39" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="Q22" s="39" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="R22" s="39" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="S22" s="39" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="T22" s="39" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="U22" s="39" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="V22" s="39" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="W22" s="39" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="X22" s="39" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="Y22" s="39" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="Z22" s="39" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AA22" s="39" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AB22" s="39" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AC22" s="39" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AD22" s="39" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AE22" s="39" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AF22" s="39" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AG22" s="39" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AH22" s="39" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AI22" s="39" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AJ22" s="39" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AK22" s="39" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AL22" s="39" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:38" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>660</v>
+      </c>
+      <c r="C23" s="35" t="s">
+        <v>661</v>
+      </c>
+      <c r="D23" s="35"/>
+      <c r="E23" s="36" t="str">
+        <f>IFERROR(E13/(E12-E13),"")</f>
+        <v/>
+      </c>
+      <c r="F23" s="36" t="str">
+        <f t="shared" ref="F23:AK23" si="6">IFERROR(F13/(F12-F13),"")</f>
+        <v/>
+      </c>
+      <c r="G23" s="36" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="H23" s="36" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I23" s="36">
+        <f t="shared" si="6"/>
+        <v>0.33890236872439872</v>
+      </c>
+      <c r="J23" s="36" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="K23" s="36" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="L23" s="36" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="M23" s="36" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="N23" s="36" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O23" s="36" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="P23" s="36" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Q23" s="36" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="R23" s="36" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="S23" s="36" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="T23" s="36" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="U23" s="36" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="V23" s="36" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="W23" s="36" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="X23" s="36" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Y23" s="36" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Z23" s="36" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="AA23" s="36" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="AB23" s="36" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="AC23" s="36" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="AD23" s="36" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="AE23" s="36" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="AF23" s="36" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="AG23" s="36" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="AH23" s="36" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="AI23" s="36" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="AJ23" s="36" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="AK23" s="36">
+        <f t="shared" si="6"/>
+        <v>0.64433402660331207</v>
+      </c>
+    </row>
+    <row r="24" spans="1:38" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>662</v>
+      </c>
+      <c r="B24" t="s">
+        <v>663</v>
+      </c>
+      <c r="C24" s="37" t="s">
+        <v>664</v>
+      </c>
+      <c r="D24" s="37"/>
+      <c r="E24" s="40" t="str">
+        <f>IFERROR(IF(E10="","",IF(E10=0,"",E10/E4)),"")</f>
+        <v/>
+      </c>
+      <c r="F24" s="40" t="str">
+        <f t="shared" ref="F24:AK24" si="7">IFERROR(IF(F10="","",IF(F10=0,"",F10/F4)),"")</f>
+        <v/>
+      </c>
+      <c r="G24" s="40" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="H24" s="40" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="I24" s="40" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="J24" s="40" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="K24" s="40" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="L24" s="40" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="M24" s="40" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="N24" s="40" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="O24" s="40" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P24" s="40" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="Q24" s="40" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="R24" s="40" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="S24" s="40" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="T24" s="40" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="U24" s="40" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="V24" s="40" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="W24" s="40" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="X24" s="40" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="Y24" s="40" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="Z24" s="40" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="AA24" s="40" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="AB24" s="40" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="AC24" s="40" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="AD24" s="40" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="AE24" s="40" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="AF24" s="40" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="AG24" s="40" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="AH24" s="40" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="AI24" s="40" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="AJ24" s="40" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="AK24" s="40" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>665</v>
+      </c>
+      <c r="B25" t="s">
+        <v>666</v>
+      </c>
+      <c r="C25" s="35" t="s">
+        <v>643</v>
+      </c>
+      <c r="D25" s="35"/>
+      <c r="E25" s="32" t="str">
+        <f>IFERROR(IF(E14=0,"",IF(E14&lt;0,"",E14)),"")</f>
+        <v/>
+      </c>
+      <c r="F25" s="32" t="str">
+        <f t="shared" ref="F25:AK25" si="8">IFERROR(IF(F14=0,"",IF(F14&lt;0,"",F14)),"")</f>
+        <v/>
+      </c>
+      <c r="G25" s="32" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="H25" s="32" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="I25" s="32" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="J25" s="32" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="K25" s="32" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="L25" s="32" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="M25" s="32" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="N25" s="32" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="O25" s="32" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="P25" s="32" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="Q25" s="32" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="R25" s="32" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="S25" s="32" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="T25" s="32" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="U25" s="32" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="V25" s="32" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="W25" s="32" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="X25" s="32" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="Y25" s="32" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="Z25" s="32" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="AA25" s="32" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="AB25" s="32" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="AC25" s="32" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="AD25" s="32" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="AE25" s="32" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="AF25" s="32" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="AG25" s="32" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="AH25" s="32" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="AI25" s="32" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="AJ25" s="32" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="AK25" s="32" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:38" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>667</v>
+      </c>
+      <c r="C26" s="35" t="s">
+        <v>668</v>
+      </c>
+      <c r="D26" s="35"/>
+      <c r="E26" s="39" t="str">
+        <f>IFERROR(IF(E25/E4=0, "",E25/E4),"")</f>
+        <v/>
+      </c>
+      <c r="F26" s="39" t="str">
+        <f t="shared" ref="F26:AK26" si="9">IFERROR(IF(F25/F4=0, "",F25/F4),"")</f>
+        <v/>
+      </c>
+      <c r="G26" s="39" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="H26" s="39" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="I26" s="39" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="J26" s="39" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="K26" s="39" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L26" s="39" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="M26" s="39" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="N26" s="39" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="O26" s="39" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="P26" s="39" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="Q26" s="39" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="R26" s="39" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="S26" s="39" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="T26" s="39" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="U26" s="39" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="V26" s="39" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="W26" s="39" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="X26" s="39" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="Y26" s="39" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="Z26" s="39" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AA26" s="39" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AB26" s="39" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AC26" s="39" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AD26" s="39" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AE26" s="39" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AF26" s="39" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AG26" s="39" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AH26" s="39" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AI26" s="39" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AJ26" s="39" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AK26" s="39" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="C27" s="41"/>
+      <c r="D27" s="41"/>
+    </row>
+    <row r="28" spans="1:38" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B28" s="42" t="s">
+        <v>669</v>
+      </c>
+      <c r="C28" s="41"/>
+      <c r="D28" s="41"/>
+    </row>
+    <row r="29" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>670</v>
+      </c>
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
+    </row>
+    <row r="30" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="C30" s="41"/>
+      <c r="D30" s="41"/>
+    </row>
+    <row r="31" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="C31" s="41"/>
+      <c r="D31" s="41"/>
+    </row>
+    <row r="32" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="C32" s="43"/>
+      <c r="D32" s="43"/>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C33" s="43"/>
+      <c r="D33" s="43"/>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C34" s="43"/>
+      <c r="D34" s="43"/>
+    </row>
+    <row r="35" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C35" s="43"/>
+      <c r="D35" s="43"/>
+    </row>
+    <row r="36" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C36" s="43"/>
+      <c r="D36" s="43"/>
+    </row>
+    <row r="37" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C37" s="43"/>
+      <c r="D37" s="43"/>
+    </row>
+    <row r="38" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C38" s="43"/>
+      <c r="D38" s="43"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M102"/>
@@ -32757,7 +35990,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>

</xml_diff>